<commit_message>
df for review 0726 12:58
Seb, can you check the file 'dataset cleaning. R' , examine the current variables of each observation (indicators) and let me which one is labeled incorrectly? you can just write a text to me, i will correct the coding

Thanks
</commit_message>
<xml_diff>
--- a/Dataset_Proposal.xlsx
+++ b/Dataset_Proposal.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\p33\20220726\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\p33\P33-DEI-dashboard-project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E8F3B3E9-8730-4E4C-86B6-FCC0236FFAFA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AA087245-B92F-468E-88F1-068CC5911706}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{3F84269C-659D-46D1-9BF0-F3F77B9F2E03}"/>
+    <workbookView xWindow="30" yWindow="30" windowWidth="28770" windowHeight="15570" xr2:uid="{3F84269C-659D-46D1-9BF0-F3F77B9F2E03}"/>
   </bookViews>
   <sheets>
     <sheet name="dataset structure" sheetId="1" r:id="rId1"/>
@@ -1091,41 +1091,41 @@
     <xf numFmtId="0" fontId="5" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1491,8 +1491,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{449FC769-74E3-46E2-872E-F46630CBECB7}">
   <dimension ref="A1:AH20"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="B24" sqref="B24"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="J14" sqref="J14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -1520,27 +1520,27 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:34" ht="57" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="46" t="s">
+      <c r="A1" s="41" t="s">
         <v>72</v>
       </c>
-      <c r="B1" s="46"/>
-      <c r="C1" s="46"/>
-      <c r="D1" s="46"/>
-      <c r="E1" s="46"/>
-      <c r="F1" s="46"/>
-      <c r="G1" s="46"/>
-      <c r="H1" s="46"/>
-      <c r="I1" s="46"/>
-      <c r="J1" s="46"/>
-      <c r="K1" s="46"/>
-      <c r="L1" s="46"/>
-      <c r="M1" s="46"/>
-      <c r="N1" s="46"/>
-      <c r="O1" s="46"/>
-      <c r="P1" s="46"/>
-      <c r="Q1" s="46"/>
-      <c r="R1" s="46"/>
-      <c r="S1" s="46"/>
+      <c r="B1" s="41"/>
+      <c r="C1" s="41"/>
+      <c r="D1" s="41"/>
+      <c r="E1" s="41"/>
+      <c r="F1" s="41"/>
+      <c r="G1" s="41"/>
+      <c r="H1" s="41"/>
+      <c r="I1" s="41"/>
+      <c r="J1" s="41"/>
+      <c r="K1" s="41"/>
+      <c r="L1" s="41"/>
+      <c r="M1" s="41"/>
+      <c r="N1" s="41"/>
+      <c r="O1" s="41"/>
+      <c r="P1" s="41"/>
+      <c r="Q1" s="41"/>
+      <c r="R1" s="41"/>
+      <c r="S1" s="41"/>
     </row>
     <row r="2" spans="1:34" ht="57" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A2" s="1"/>
@@ -1580,142 +1580,142 @@
     </row>
     <row r="3" spans="1:34" ht="57" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A3" s="1"/>
-      <c r="B3" s="41" t="s">
+      <c r="B3" s="46" t="s">
         <v>29</v>
       </c>
-      <c r="C3" s="42"/>
-      <c r="D3" s="42"/>
-      <c r="E3" s="42"/>
-      <c r="F3" s="42"/>
-      <c r="G3" s="42"/>
-      <c r="H3" s="42"/>
-      <c r="I3" s="42"/>
-      <c r="J3" s="42"/>
-      <c r="K3" s="42"/>
-      <c r="L3" s="42"/>
-      <c r="M3" s="42"/>
-      <c r="N3" s="42"/>
-      <c r="O3" s="42"/>
-      <c r="P3" s="42"/>
-      <c r="Q3" s="42"/>
-      <c r="R3" s="42"/>
-      <c r="S3" s="43"/>
-      <c r="T3" s="41" t="s">
+      <c r="C3" s="47"/>
+      <c r="D3" s="47"/>
+      <c r="E3" s="47"/>
+      <c r="F3" s="47"/>
+      <c r="G3" s="47"/>
+      <c r="H3" s="47"/>
+      <c r="I3" s="47"/>
+      <c r="J3" s="47"/>
+      <c r="K3" s="47"/>
+      <c r="L3" s="47"/>
+      <c r="M3" s="47"/>
+      <c r="N3" s="47"/>
+      <c r="O3" s="47"/>
+      <c r="P3" s="47"/>
+      <c r="Q3" s="47"/>
+      <c r="R3" s="47"/>
+      <c r="S3" s="48"/>
+      <c r="T3" s="46" t="s">
         <v>35</v>
       </c>
-      <c r="U3" s="42"/>
-      <c r="V3" s="42"/>
-      <c r="W3" s="42"/>
-      <c r="X3" s="42"/>
-      <c r="Y3" s="42"/>
-      <c r="Z3" s="42"/>
-      <c r="AA3" s="42"/>
-      <c r="AB3" s="42"/>
-      <c r="AC3" s="42"/>
-      <c r="AD3" s="42"/>
-      <c r="AE3" s="42"/>
-      <c r="AF3" s="42"/>
-      <c r="AG3" s="42"/>
-      <c r="AH3" s="43"/>
+      <c r="U3" s="47"/>
+      <c r="V3" s="47"/>
+      <c r="W3" s="47"/>
+      <c r="X3" s="47"/>
+      <c r="Y3" s="47"/>
+      <c r="Z3" s="47"/>
+      <c r="AA3" s="47"/>
+      <c r="AB3" s="47"/>
+      <c r="AC3" s="47"/>
+      <c r="AD3" s="47"/>
+      <c r="AE3" s="47"/>
+      <c r="AF3" s="47"/>
+      <c r="AG3" s="47"/>
+      <c r="AH3" s="48"/>
     </row>
     <row r="4" spans="1:34" ht="22.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A4" s="1"/>
       <c r="B4" s="23" t="s">
         <v>44</v>
       </c>
-      <c r="C4" s="41" t="s">
+      <c r="C4" s="46" t="s">
         <v>54</v>
       </c>
-      <c r="D4" s="42"/>
-      <c r="E4" s="42"/>
-      <c r="F4" s="42"/>
-      <c r="G4" s="42"/>
-      <c r="H4" s="42"/>
-      <c r="I4" s="42"/>
-      <c r="J4" s="43"/>
-      <c r="K4" s="41" t="s">
+      <c r="D4" s="47"/>
+      <c r="E4" s="47"/>
+      <c r="F4" s="47"/>
+      <c r="G4" s="47"/>
+      <c r="H4" s="47"/>
+      <c r="I4" s="47"/>
+      <c r="J4" s="48"/>
+      <c r="K4" s="46" t="s">
         <v>57</v>
       </c>
-      <c r="L4" s="42"/>
-      <c r="M4" s="42"/>
-      <c r="N4" s="42"/>
-      <c r="O4" s="42"/>
-      <c r="P4" s="43"/>
-      <c r="Q4" s="42" t="s">
+      <c r="L4" s="47"/>
+      <c r="M4" s="47"/>
+      <c r="N4" s="47"/>
+      <c r="O4" s="47"/>
+      <c r="P4" s="48"/>
+      <c r="Q4" s="47" t="s">
         <v>65</v>
       </c>
-      <c r="R4" s="42"/>
-      <c r="S4" s="42"/>
-      <c r="T4" s="41" t="s">
+      <c r="R4" s="47"/>
+      <c r="S4" s="47"/>
+      <c r="T4" s="46" t="s">
         <v>55</v>
       </c>
-      <c r="U4" s="42"/>
-      <c r="V4" s="42"/>
-      <c r="W4" s="42"/>
-      <c r="X4" s="43"/>
-      <c r="Y4" s="41" t="s">
+      <c r="U4" s="47"/>
+      <c r="V4" s="47"/>
+      <c r="W4" s="47"/>
+      <c r="X4" s="48"/>
+      <c r="Y4" s="46" t="s">
         <v>64</v>
       </c>
-      <c r="Z4" s="42"/>
-      <c r="AA4" s="42"/>
-      <c r="AB4" s="42"/>
-      <c r="AC4" s="43"/>
-      <c r="AD4" s="42" t="s">
+      <c r="Z4" s="47"/>
+      <c r="AA4" s="47"/>
+      <c r="AB4" s="47"/>
+      <c r="AC4" s="48"/>
+      <c r="AD4" s="47" t="s">
         <v>67</v>
       </c>
-      <c r="AE4" s="42"/>
-      <c r="AF4" s="42"/>
-      <c r="AG4" s="42"/>
-      <c r="AH4" s="43"/>
+      <c r="AE4" s="47"/>
+      <c r="AF4" s="47"/>
+      <c r="AG4" s="47"/>
+      <c r="AH4" s="48"/>
     </row>
     <row r="5" spans="1:34" ht="44.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B5" s="4" t="s">
         <v>34</v>
       </c>
-      <c r="C5" s="38" t="s">
+      <c r="C5" s="42" t="s">
         <v>23</v>
       </c>
-      <c r="D5" s="39"/>
-      <c r="E5" s="39"/>
-      <c r="F5" s="39"/>
-      <c r="G5" s="39"/>
-      <c r="H5" s="39"/>
-      <c r="I5" s="39"/>
-      <c r="J5" s="40"/>
-      <c r="K5" s="47" t="s">
+      <c r="D5" s="43"/>
+      <c r="E5" s="43"/>
+      <c r="F5" s="43"/>
+      <c r="G5" s="43"/>
+      <c r="H5" s="43"/>
+      <c r="I5" s="43"/>
+      <c r="J5" s="44"/>
+      <c r="K5" s="45" t="s">
         <v>30</v>
       </c>
-      <c r="L5" s="39"/>
-      <c r="M5" s="39"/>
-      <c r="N5" s="39"/>
-      <c r="O5" s="39"/>
-      <c r="P5" s="40"/>
-      <c r="Q5" s="38" t="s">
+      <c r="L5" s="43"/>
+      <c r="M5" s="43"/>
+      <c r="N5" s="43"/>
+      <c r="O5" s="43"/>
+      <c r="P5" s="44"/>
+      <c r="Q5" s="42" t="s">
         <v>56</v>
       </c>
-      <c r="R5" s="39"/>
-      <c r="S5" s="40"/>
-      <c r="T5" s="38" t="s">
+      <c r="R5" s="43"/>
+      <c r="S5" s="44"/>
+      <c r="T5" s="42" t="s">
         <v>43</v>
       </c>
-      <c r="U5" s="39"/>
-      <c r="V5" s="39"/>
-      <c r="W5" s="39"/>
-      <c r="X5" s="40"/>
-      <c r="Y5" s="38" t="s">
+      <c r="U5" s="43"/>
+      <c r="V5" s="43"/>
+      <c r="W5" s="43"/>
+      <c r="X5" s="44"/>
+      <c r="Y5" s="42" t="s">
         <v>56</v>
       </c>
-      <c r="Z5" s="39"/>
-      <c r="AA5" s="39"/>
-      <c r="AB5" s="39"/>
-      <c r="AC5" s="40"/>
-      <c r="AD5" s="44" t="s">
+      <c r="Z5" s="43"/>
+      <c r="AA5" s="43"/>
+      <c r="AB5" s="43"/>
+      <c r="AC5" s="44"/>
+      <c r="AD5" s="49" t="s">
         <v>66</v>
       </c>
-      <c r="AE5" s="44"/>
-      <c r="AF5" s="44"/>
-      <c r="AG5" s="44"/>
-      <c r="AH5" s="45"/>
+      <c r="AE5" s="49"/>
+      <c r="AF5" s="49"/>
+      <c r="AG5" s="49"/>
+      <c r="AH5" s="50"/>
     </row>
     <row r="6" spans="1:34" s="31" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B6" s="32" t="s">
@@ -2172,11 +2172,6 @@
     </row>
   </sheetData>
   <mergeCells count="15">
-    <mergeCell ref="A1:S1"/>
-    <mergeCell ref="C5:J5"/>
-    <mergeCell ref="K5:P5"/>
-    <mergeCell ref="Q5:S5"/>
-    <mergeCell ref="B3:S3"/>
     <mergeCell ref="T5:X5"/>
     <mergeCell ref="Y5:AC5"/>
     <mergeCell ref="T3:AH3"/>
@@ -2187,6 +2182,11 @@
     <mergeCell ref="T4:X4"/>
     <mergeCell ref="Y4:AC4"/>
     <mergeCell ref="AD4:AH4"/>
+    <mergeCell ref="A1:S1"/>
+    <mergeCell ref="C5:J5"/>
+    <mergeCell ref="K5:P5"/>
+    <mergeCell ref="Q5:S5"/>
+    <mergeCell ref="B3:S3"/>
   </mergeCells>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2197,8 +2197,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5B49C3A3-35BB-4FB3-92A8-99679C41C11D}">
   <dimension ref="A1:G58"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A24" sqref="A24:A29"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -3567,766 +3567,766 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A1" s="48" t="s">
+      <c r="A1" s="38" t="s">
         <v>142</v>
       </c>
-      <c r="B1" s="48" t="s">
+      <c r="B1" s="38" t="s">
         <v>74</v>
       </c>
-      <c r="C1" s="48" t="s">
+      <c r="C1" s="38" t="s">
         <v>75</v>
       </c>
-      <c r="D1" s="48" t="s">
+      <c r="D1" s="38" t="s">
         <v>76</v>
       </c>
-      <c r="E1" s="48" t="s">
+      <c r="E1" s="38" t="s">
         <v>77</v>
       </c>
-      <c r="F1" s="48" t="s">
+      <c r="F1" s="38" t="s">
         <v>78</v>
       </c>
-      <c r="G1" s="48" t="s">
+      <c r="G1" s="38" t="s">
         <v>79</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A2" s="48" t="s">
+      <c r="A2" s="38" t="s">
         <v>143</v>
       </c>
-      <c r="B2" s="48">
+      <c r="B2" s="38">
         <f t="shared" ref="B2:B7" si="0">SUM(C2:F2)</f>
         <v>22252</v>
       </c>
-      <c r="C2" s="48">
+      <c r="C2" s="38">
         <v>8275</v>
       </c>
-      <c r="D2" s="48">
+      <c r="D2" s="38">
         <v>10392</v>
       </c>
-      <c r="E2" s="48">
+      <c r="E2" s="38">
         <v>2501</v>
       </c>
-      <c r="F2" s="48">
+      <c r="F2" s="38">
         <v>1084</v>
       </c>
-      <c r="G2" s="49" t="s">
+      <c r="G2" s="39" t="s">
         <v>86</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A3" s="48" t="s">
+      <c r="A3" s="38" t="s">
         <v>144</v>
       </c>
-      <c r="B3" s="48">
+      <c r="B3" s="38">
         <f t="shared" si="0"/>
         <v>25465</v>
       </c>
-      <c r="C3" s="48">
+      <c r="C3" s="38">
         <v>9376</v>
       </c>
-      <c r="D3" s="48">
+      <c r="D3" s="38">
         <v>12500</v>
       </c>
-      <c r="E3" s="48">
+      <c r="E3" s="38">
         <v>2566</v>
       </c>
-      <c r="F3" s="48">
+      <c r="F3" s="38">
         <v>1023</v>
       </c>
-      <c r="G3" s="49" t="s">
+      <c r="G3" s="39" t="s">
         <v>86</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A4" s="48" t="s">
+      <c r="A4" s="38" t="s">
         <v>145</v>
       </c>
-      <c r="B4" s="48">
+      <c r="B4" s="38">
         <f t="shared" si="0"/>
         <v>205654</v>
       </c>
-      <c r="C4" s="48">
+      <c r="C4" s="38">
         <v>76478</v>
       </c>
-      <c r="D4" s="48">
+      <c r="D4" s="38">
         <v>95809</v>
       </c>
-      <c r="E4" s="50">
+      <c r="E4" s="40">
         <v>23965</v>
       </c>
-      <c r="F4" s="48">
+      <c r="F4" s="38">
         <v>9402</v>
       </c>
-      <c r="G4" s="49" t="s">
+      <c r="G4" s="39" t="s">
         <v>86</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A5" s="48" t="s">
+      <c r="A5" s="38" t="s">
         <v>146</v>
       </c>
-      <c r="B5" s="48">
+      <c r="B5" s="38">
         <f t="shared" si="0"/>
         <v>25552</v>
       </c>
-      <c r="C5" s="48">
+      <c r="C5" s="38">
         <v>9285</v>
       </c>
-      <c r="D5" s="48">
+      <c r="D5" s="38">
         <v>12923</v>
       </c>
-      <c r="E5" s="48">
+      <c r="E5" s="38">
         <v>2306</v>
       </c>
-      <c r="F5" s="48">
+      <c r="F5" s="38">
         <v>1038</v>
       </c>
-      <c r="G5" s="49" t="s">
+      <c r="G5" s="39" t="s">
         <v>86</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A6" s="48" t="s">
+      <c r="A6" s="38" t="s">
         <v>147</v>
       </c>
-      <c r="B6" s="48">
+      <c r="B6" s="38">
         <f t="shared" si="0"/>
         <v>26053</v>
       </c>
-      <c r="C6" s="48">
+      <c r="C6" s="38">
         <v>9608</v>
       </c>
-      <c r="D6" s="48">
+      <c r="D6" s="38">
         <v>13039</v>
       </c>
-      <c r="E6" s="48">
+      <c r="E6" s="38">
         <v>2404</v>
       </c>
-      <c r="F6" s="48">
+      <c r="F6" s="38">
         <v>1002</v>
       </c>
-      <c r="G6" s="49" t="s">
+      <c r="G6" s="39" t="s">
         <v>86</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A7" s="48" t="s">
+      <c r="A7" s="38" t="s">
         <v>148</v>
       </c>
-      <c r="B7" s="48">
+      <c r="B7" s="38">
         <f t="shared" si="0"/>
         <v>26118</v>
       </c>
-      <c r="C7" s="48">
+      <c r="C7" s="38">
         <v>9535</v>
       </c>
-      <c r="D7" s="48">
+      <c r="D7" s="38">
         <v>12869</v>
       </c>
-      <c r="E7" s="48">
+      <c r="E7" s="38">
         <v>2623</v>
       </c>
-      <c r="F7" s="48">
+      <c r="F7" s="38">
         <v>1091</v>
       </c>
-      <c r="G7" s="49" t="s">
+      <c r="G7" s="39" t="s">
         <v>86</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A8" s="48" t="s">
+      <c r="A8" s="38" t="s">
         <v>149</v>
       </c>
-      <c r="B8" s="48">
+      <c r="B8" s="38">
         <f>B9-SUM(B5:B7)</f>
         <v>24694</v>
       </c>
-      <c r="C8" s="48">
+      <c r="C8" s="38">
         <v>8775</v>
       </c>
-      <c r="D8" s="48">
+      <c r="D8" s="38">
         <v>12397</v>
       </c>
-      <c r="E8" s="48">
+      <c r="E8" s="38">
         <v>2391</v>
       </c>
-      <c r="F8" s="48">
+      <c r="F8" s="38">
         <v>1131</v>
       </c>
-      <c r="G8" s="49" t="s">
+      <c r="G8" s="39" t="s">
         <v>86</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A9" s="48" t="s">
+      <c r="A9" s="38" t="s">
         <v>150</v>
       </c>
-      <c r="B9" s="48">
+      <c r="B9" s="38">
         <f>SUM(C9:F9)</f>
         <v>102417</v>
       </c>
-      <c r="C9" s="48">
+      <c r="C9" s="38">
         <f>SUM(C5:C8)</f>
         <v>37203</v>
       </c>
-      <c r="D9" s="48">
+      <c r="D9" s="38">
         <f t="shared" ref="D9:F9" si="1">SUM(D5:D8)</f>
         <v>51228</v>
       </c>
-      <c r="E9" s="48">
+      <c r="E9" s="38">
         <f t="shared" si="1"/>
         <v>9724</v>
       </c>
-      <c r="F9" s="48">
+      <c r="F9" s="38">
         <f t="shared" si="1"/>
         <v>4262</v>
       </c>
-      <c r="G9" s="49" t="s">
+      <c r="G9" s="39" t="s">
         <v>86</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A10" s="48" t="s">
+      <c r="A10" s="38" t="s">
         <v>151</v>
       </c>
-      <c r="B10" s="48">
+      <c r="B10" s="38">
         <f>SUM(C10:F10)</f>
         <v>139687</v>
       </c>
-      <c r="C10" s="48">
+      <c r="C10" s="38">
         <v>24193</v>
       </c>
-      <c r="D10" s="48">
+      <c r="D10" s="38">
         <v>39877</v>
       </c>
-      <c r="E10" s="48">
+      <c r="E10" s="38">
         <v>68100</v>
       </c>
-      <c r="F10" s="48">
+      <c r="F10" s="38">
         <v>7517</v>
       </c>
-      <c r="G10" s="49" t="s">
+      <c r="G10" s="39" t="s">
         <v>96</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A11" s="48" t="s">
+      <c r="A11" s="38" t="s">
         <v>92</v>
       </c>
-      <c r="B11" s="48">
+      <c r="B11" s="38">
         <f>SUM(C11:F11)</f>
         <v>133178</v>
       </c>
-      <c r="C11" s="48">
+      <c r="C11" s="38">
         <v>20880</v>
       </c>
-      <c r="D11" s="48">
+      <c r="D11" s="38">
         <v>34946</v>
       </c>
-      <c r="E11" s="48">
+      <c r="E11" s="38">
         <v>69614</v>
       </c>
-      <c r="F11" s="48">
+      <c r="F11" s="38">
         <v>7738</v>
       </c>
-      <c r="G11" s="49" t="s">
+      <c r="G11" s="39" t="s">
         <v>96</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A12" s="48" t="s">
+      <c r="A12" s="38" t="s">
         <v>152</v>
       </c>
-      <c r="B12" s="48">
+      <c r="B12" s="38">
         <v>577000</v>
       </c>
-      <c r="C12" s="48">
+      <c r="C12" s="38">
         <v>103860</v>
       </c>
-      <c r="D12" s="48">
+      <c r="D12" s="38">
         <v>155790</v>
       </c>
-      <c r="E12" s="48">
+      <c r="E12" s="38">
         <v>282730</v>
       </c>
-      <c r="F12" s="48">
+      <c r="F12" s="38">
         <v>28850</v>
       </c>
-      <c r="G12" s="49" t="s">
+      <c r="G12" s="39" t="s">
         <v>96</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A13" s="48" t="s">
+      <c r="A13" s="38" t="s">
         <v>153</v>
       </c>
-      <c r="B13" s="48">
+      <c r="B13" s="38">
         <v>233051</v>
       </c>
-      <c r="C13" s="48">
+      <c r="C13" s="38">
         <v>27966</v>
       </c>
-      <c r="D13" s="48">
+      <c r="D13" s="38">
         <v>51271</v>
       </c>
-      <c r="E13" s="48">
+      <c r="E13" s="38">
         <v>130509</v>
       </c>
-      <c r="F13" s="48">
+      <c r="F13" s="38">
         <v>23305</v>
       </c>
-      <c r="G13" s="49" t="s">
+      <c r="G13" s="39" t="s">
         <v>86</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A14" s="48" t="s">
+      <c r="A14" s="38" t="s">
         <v>154</v>
       </c>
-      <c r="B14" s="48">
+      <c r="B14" s="38">
         <f>B13-'[1]Raw Data'!B14</f>
         <v>230098</v>
       </c>
-      <c r="C14" s="48">
+      <c r="C14" s="38">
         <f>C13-'[1]Raw Data'!C14</f>
         <v>27773</v>
       </c>
-      <c r="D14" s="48">
+      <c r="D14" s="38">
         <f>D13-'[1]Raw Data'!D14</f>
         <v>50822</v>
       </c>
-      <c r="E14" s="48">
+      <c r="E14" s="38">
         <f>E13-'[1]Raw Data'!E14</f>
         <v>129070</v>
       </c>
-      <c r="F14" s="48">
+      <c r="F14" s="38">
         <f>F13-'[1]Raw Data'!F14</f>
         <v>22433</v>
       </c>
-      <c r="G14" s="49" t="s">
+      <c r="G14" s="39" t="s">
         <v>107</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A15" s="48" t="s">
+      <c r="A15" s="38" t="s">
         <v>155</v>
       </c>
-      <c r="B15" s="48">
+      <c r="B15" s="38">
         <f>31520 +29503</f>
         <v>61023</v>
       </c>
-      <c r="C15" s="48">
+      <c r="C15" s="38">
         <v>6102</v>
       </c>
-      <c r="D15" s="48">
+      <c r="D15" s="38">
         <v>11594</v>
       </c>
-      <c r="E15" s="48">
+      <c r="E15" s="38">
         <v>37224</v>
       </c>
-      <c r="F15" s="48">
+      <c r="F15" s="38">
         <v>6713</v>
       </c>
-      <c r="G15" s="49" t="s">
+      <c r="G15" s="39" t="s">
         <v>86</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A16" s="48" t="s">
+      <c r="A16" s="38" t="s">
         <v>156</v>
       </c>
-      <c r="B16" s="48">
+      <c r="B16" s="38">
         <v>2700000</v>
       </c>
-      <c r="C16" s="48">
+      <c r="C16" s="38">
         <v>810000</v>
       </c>
-      <c r="D16" s="48">
+      <c r="D16" s="38">
         <v>783000</v>
       </c>
-      <c r="E16" s="48">
+      <c r="E16" s="38">
         <v>810000</v>
       </c>
-      <c r="F16" s="48">
+      <c r="F16" s="38">
         <v>297000</v>
       </c>
-      <c r="G16" s="49" t="s">
+      <c r="G16" s="39" t="s">
         <v>96</v>
       </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A17" s="48" t="s">
+      <c r="A17" s="38" t="s">
         <v>157</v>
       </c>
-      <c r="B17" s="48">
+      <c r="B17" s="38">
         <f>SUM(C17:F17)</f>
         <v>1151971</v>
       </c>
-      <c r="C17" s="48">
+      <c r="C17" s="38">
         <f>185882</f>
         <v>185882</v>
       </c>
-      <c r="D17" s="48">
+      <c r="D17" s="38">
         <f>261730</f>
         <v>261730</v>
       </c>
-      <c r="E17" s="48">
+      <c r="E17" s="38">
         <f>633474</f>
         <v>633474</v>
       </c>
-      <c r="F17" s="48">
+      <c r="F17" s="38">
         <f>70885</f>
         <v>70885</v>
       </c>
-      <c r="G17" s="49" t="s">
+      <c r="G17" s="39" t="s">
         <v>86</v>
       </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A18" s="48" t="s">
+      <c r="A18" s="38" t="s">
         <v>158</v>
       </c>
-      <c r="B18" s="48">
+      <c r="B18" s="38">
         <v>5438637</v>
       </c>
-      <c r="C18" s="48">
+      <c r="C18" s="38">
         <v>905408</v>
       </c>
-      <c r="D18" s="48">
+      <c r="D18" s="38">
         <v>1212984</v>
       </c>
-      <c r="E18" s="48">
+      <c r="E18" s="38">
         <v>2888593</v>
       </c>
-      <c r="F18" s="48">
+      <c r="F18" s="38">
         <v>431652</v>
       </c>
-      <c r="G18" s="49" t="s">
+      <c r="G18" s="39" t="s">
         <v>86</v>
       </c>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A19" s="48" t="s">
+      <c r="A19" s="38" t="s">
         <v>159</v>
       </c>
-      <c r="B19" s="48">
+      <c r="B19" s="38">
         <f>168454+352094 +635486 +167208</f>
         <v>1323242</v>
       </c>
-      <c r="C19" s="48">
+      <c r="C19" s="38">
         <f>168454</f>
         <v>168454</v>
       </c>
-      <c r="D19" s="48">
+      <c r="D19" s="38">
         <f>352894</f>
         <v>352894</v>
       </c>
-      <c r="E19" s="48">
+      <c r="E19" s="38">
         <f>635486</f>
         <v>635486</v>
       </c>
-      <c r="F19" s="48">
+      <c r="F19" s="38">
         <f>167208</f>
         <v>167208</v>
       </c>
-      <c r="G19" s="49" t="s">
+      <c r="G19" s="39" t="s">
         <v>86</v>
       </c>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A20" s="48" t="s">
+      <c r="A20" s="38" t="s">
         <v>160</v>
       </c>
-      <c r="B20" s="48">
+      <c r="B20" s="38">
         <v>23093</v>
       </c>
-      <c r="C20" s="48">
+      <c r="C20" s="38">
         <v>7855</v>
       </c>
-      <c r="D20" s="48">
+      <c r="D20" s="38">
         <v>11419</v>
       </c>
-      <c r="E20" s="48">
+      <c r="E20" s="38">
         <v>2278</v>
       </c>
-      <c r="F20" s="48">
+      <c r="F20" s="38">
         <v>1090</v>
       </c>
-      <c r="G20" s="49" t="s">
+      <c r="G20" s="39" t="s">
         <v>86</v>
       </c>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A21" s="48" t="s">
+      <c r="A21" s="38" t="s">
         <v>161</v>
       </c>
-      <c r="B21" s="48">
+      <c r="B21" s="38">
         <f>SUM(C21:F21)</f>
         <v>141564</v>
       </c>
-      <c r="C21" s="48">
+      <c r="C21" s="38">
         <v>22590</v>
       </c>
-      <c r="D21" s="48">
+      <c r="D21" s="38">
         <v>42168.000000000007</v>
       </c>
-      <c r="E21" s="48">
+      <c r="E21" s="38">
         <v>69276</v>
       </c>
-      <c r="F21" s="48">
+      <c r="F21" s="38">
         <v>7530</v>
       </c>
-      <c r="G21" s="49" t="s">
+      <c r="G21" s="39" t="s">
         <v>86</v>
       </c>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A22" s="48" t="s">
+      <c r="A22" s="38" t="s">
         <v>162</v>
       </c>
-      <c r="B22" s="48">
+      <c r="B22" s="38">
         <f>SUM(C22:F22)</f>
         <v>137376</v>
       </c>
-      <c r="C22" s="48">
+      <c r="C22" s="38">
         <v>21465</v>
       </c>
-      <c r="D22" s="48">
+      <c r="D22" s="38">
         <v>38637</v>
       </c>
-      <c r="E22" s="48">
+      <c r="E22" s="38">
         <v>68688</v>
       </c>
-      <c r="F22" s="48">
+      <c r="F22" s="38">
         <v>8586</v>
       </c>
-      <c r="G22" s="49" t="s">
+      <c r="G22" s="39" t="s">
         <v>86</v>
       </c>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A23" s="48" t="s">
+      <c r="A23" s="38" t="s">
         <v>163</v>
       </c>
-      <c r="B23" s="48">
+      <c r="B23" s="38">
         <f>SUM(C23:F23)</f>
         <v>1764</v>
       </c>
-      <c r="C23" s="48">
+      <c r="C23" s="38">
         <v>648</v>
       </c>
-      <c r="D23" s="48">
+      <c r="D23" s="38">
         <v>864</v>
       </c>
-      <c r="E23" s="48">
+      <c r="E23" s="38">
         <v>180</v>
       </c>
-      <c r="F23" s="48">
+      <c r="F23" s="38">
         <v>72</v>
       </c>
-      <c r="G23" s="49" t="s">
+      <c r="G23" s="39" t="s">
         <v>86</v>
       </c>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A24" s="48" t="s">
+      <c r="A24" s="38" t="s">
         <v>164</v>
       </c>
-      <c r="B24" s="48">
+      <c r="B24" s="38">
         <v>1700</v>
       </c>
-      <c r="C24" s="48">
+      <c r="C24" s="38">
         <f>0.38*B24</f>
         <v>646</v>
       </c>
-      <c r="D24" s="48">
+      <c r="D24" s="38">
         <f>0.49*B24</f>
         <v>833</v>
       </c>
-      <c r="E24" s="48">
+      <c r="E24" s="38">
         <f>0.08*B24</f>
         <v>136</v>
       </c>
-      <c r="F24" s="48">
+      <c r="F24" s="38">
         <f>0.05*B24</f>
         <v>85</v>
       </c>
-      <c r="G24" s="49" t="s">
+      <c r="G24" s="39" t="s">
         <v>86</v>
       </c>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A25" s="48" t="s">
+      <c r="A25" s="38" t="s">
         <v>165</v>
       </c>
-      <c r="B25" s="48">
+      <c r="B25" s="38">
         <f>SUM(C25:F25)</f>
         <v>3700000</v>
       </c>
-      <c r="C25" s="48">
+      <c r="C25" s="38">
         <v>600000</v>
       </c>
-      <c r="D25" s="48">
+      <c r="D25" s="38">
         <v>1100000</v>
       </c>
-      <c r="E25" s="48">
+      <c r="E25" s="38">
         <v>1800000</v>
       </c>
-      <c r="F25" s="48">
+      <c r="F25" s="38">
         <v>200000</v>
       </c>
-      <c r="G25" s="49" t="s">
+      <c r="G25" s="39" t="s">
         <v>166</v>
       </c>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A26" s="48" t="s">
+      <c r="A26" s="38" t="s">
         <v>167</v>
       </c>
-      <c r="B26" s="48">
+      <c r="B26" s="38">
         <f>SUM(C26:F26)</f>
         <v>3660000</v>
       </c>
-      <c r="C26" s="48">
+      <c r="C26" s="38">
         <v>560000</v>
       </c>
-      <c r="D26" s="48">
+      <c r="D26" s="38">
         <v>1100000</v>
       </c>
-      <c r="E26" s="48">
+      <c r="E26" s="38">
         <v>1800000</v>
       </c>
-      <c r="F26" s="48">
+      <c r="F26" s="38">
         <v>200000</v>
       </c>
-      <c r="G26" s="49" t="s">
+      <c r="G26" s="39" t="s">
         <v>166</v>
       </c>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A27" s="48" t="s">
+      <c r="A27" s="38" t="s">
         <v>168</v>
       </c>
-      <c r="B27" s="48">
+      <c r="B27" s="38">
         <f>SUM(C27:F27)</f>
         <v>14748000</v>
       </c>
-      <c r="C27" s="48">
+      <c r="C27" s="38">
         <v>2274000</v>
       </c>
-      <c r="D27" s="48">
+      <c r="D27" s="38">
         <v>4345000</v>
       </c>
-      <c r="E27" s="48">
+      <c r="E27" s="38">
         <v>7202000</v>
       </c>
-      <c r="F27" s="48">
+      <c r="F27" s="38">
         <v>927000</v>
       </c>
-      <c r="G27" s="49" t="s">
+      <c r="G27" s="39" t="s">
         <v>166</v>
       </c>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A28" s="48" t="s">
+      <c r="A28" s="38" t="s">
         <v>169</v>
       </c>
-      <c r="B28" s="48">
+      <c r="B28" s="38">
         <v>330000000</v>
       </c>
-      <c r="C28" s="48">
+      <c r="C28" s="38">
         <f>0.126*B28</f>
         <v>41580000</v>
       </c>
-      <c r="D28" s="48">
+      <c r="D28" s="38">
         <f>0.186*B28</f>
         <v>61380000</v>
       </c>
-      <c r="E28" s="48">
+      <c r="E28" s="38">
         <f>0.597*B28</f>
         <v>197010000</v>
       </c>
-      <c r="F28" s="48">
+      <c r="F28" s="38">
         <f>0.059*B28</f>
         <v>19470000</v>
       </c>
-      <c r="G28" s="49" t="s">
+      <c r="G28" s="39" t="s">
         <v>166</v>
       </c>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A29" s="48" t="s">
+      <c r="A29" s="38" t="s">
         <v>170</v>
       </c>
-      <c r="B29" s="48">
+      <c r="B29" s="38">
         <f>SUM(C29:F29)</f>
         <v>185445419</v>
       </c>
-      <c r="C29" s="48">
+      <c r="C29" s="38">
         <f>25187271</f>
         <v>25187271</v>
       </c>
-      <c r="D29" s="48">
+      <c r="D29" s="38">
         <f>34381798</f>
         <v>34381798</v>
       </c>
-      <c r="E29" s="48">
+      <c r="E29" s="38">
         <f>113281506</f>
         <v>113281506</v>
       </c>
-      <c r="F29" s="48">
+      <c r="F29" s="38">
         <f>12594844</f>
         <v>12594844</v>
       </c>
-      <c r="G29" s="49" t="s">
+      <c r="G29" s="39" t="s">
         <v>86</v>
       </c>
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A30" s="48" t="s">
+      <c r="A30" s="38" t="s">
         <v>171</v>
       </c>
-      <c r="B30" s="48">
+      <c r="B30" s="38">
         <f>SUM(C30:F30)</f>
         <v>29376000</v>
       </c>
-      <c r="C30" s="48">
+      <c r="C30" s="38">
         <v>4284000</v>
       </c>
-      <c r="D30" s="48">
+      <c r="D30" s="38">
         <v>6732000</v>
       </c>
-      <c r="E30" s="48">
+      <c r="E30" s="38">
         <v>16524000.000000002</v>
       </c>
-      <c r="F30" s="48">
+      <c r="F30" s="38">
         <v>1836000</v>
       </c>
-      <c r="G30" s="49" t="s">
+      <c r="G30" s="39" t="s">
         <v>86</v>
       </c>
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A31" s="48" t="s">
+      <c r="A31" s="38" t="s">
         <v>172</v>
       </c>
-      <c r="B31" s="48">
+      <c r="B31" s="38">
         <f>SUM(C31:F31)</f>
         <v>3204450</v>
       </c>
-      <c r="C31" s="48">
+      <c r="C31" s="38">
         <v>458110</v>
       </c>
-      <c r="D31" s="48">
+      <c r="D31" s="38">
         <v>863170</v>
       </c>
-      <c r="E31" s="48">
+      <c r="E31" s="38">
         <v>1673240</v>
       </c>
-      <c r="F31" s="48">
+      <c r="F31" s="38">
         <v>209930</v>
       </c>
-      <c r="G31" s="49" t="s">
+      <c r="G31" s="39" t="s">
         <v>86</v>
       </c>
     </row>

</xml_diff>